<commit_message>
Updated master parts list
</commit_message>
<xml_diff>
--- a/Hardware/Master Parts List.xlsx
+++ b/Hardware/Master Parts List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="54">
   <si>
     <t>From</t>
   </si>
@@ -158,6 +158,24 @@
   </si>
   <si>
     <t>Need to order (can use Arduino / crystal)</t>
+  </si>
+  <si>
+    <t>IC Socket</t>
+  </si>
+  <si>
+    <t>ICS28N</t>
+  </si>
+  <si>
+    <t>3mm LED</t>
+  </si>
+  <si>
+    <t>LED3R</t>
+  </si>
+  <si>
+    <t>100R Resistor</t>
+  </si>
+  <si>
+    <t>R100R14W</t>
   </si>
 </sst>
 </file>
@@ -248,8 +266,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E16" totalsRowCount="1" tableBorderDxfId="4">
-  <autoFilter ref="A2:E15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E19" totalsRowCount="1" tableBorderDxfId="4">
+  <autoFilter ref="A2:E18"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Cat."/>
@@ -262,8 +280,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A19:E27" totalsRowCount="1">
-  <autoFilter ref="A19:E26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A22:E33" totalsRowCount="1">
+  <autoFilter ref="A22:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Cat."/>
@@ -562,7 +580,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -619,13 +637,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -636,13 +654,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1">
-        <v>0.05</v>
+        <v>0.21</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -653,118 +671,119 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <f>0.11/10*5</f>
         <v>5.4999999999999993E-2</v>
       </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="1">
+        <f>0.11/10</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C10" s="1">
         <f>0.42*4</f>
         <v>1.68</v>
       </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C11" s="1">
         <f>11.82+0.99*11.82/10.57</f>
         <v>12.927076631977295</v>
       </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1.44</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>3.27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2.48</v>
-      </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
-        <v>1.79</v>
+        <v>1.44</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
@@ -775,148 +794,148 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1">
-        <v>1.62</v>
+        <v>3.27</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2.48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.79</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C17" s="1">
         <f>6.32/2</f>
         <v>3.16</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C18" s="1">
         <f>3.2/5</f>
         <v>0.64</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D18" t="s">
         <v>3</v>
       </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="1">
-        <f>SUBTOTAL(109,Table1[Cost])</f>
-        <v>31.632076631977295</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>29</v>
+      <c r="E18" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2.31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="C19" s="1">
+        <f>SUBTOTAL(109,Table1[Cost])</f>
+        <v>31.893076631977298</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>47</v>
+      <c r="A21" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.74</v>
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1">
-        <v>0.05</v>
+        <v>2.31</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -927,63 +946,166 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>6</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B28" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C28" s="1">
         <f>0.11/10</f>
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="1">
+        <f>0.11/10</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>18</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B31" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C31" s="1">
         <v>1.44</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D31" t="s">
         <v>3</v>
       </c>
-      <c r="E25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="E31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C32" s="1">
         <v>6.14</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D32" t="s">
         <v>45</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E32" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C33" s="1">
         <f>SUBTOTAL(109,Table2[Cost])</f>
-        <v>10.901</v>
+        <v>11.161999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>